<commit_message>
finished philosophy, rates, curriculum
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Worked on the locations page; Deploy v2011.11.03.1</t>
+  </si>
+  <si>
+    <t>Rename css files; Move header and menu to JavaScript file; Started philosophy, drop shadow for float right pictures and styling</t>
+  </si>
+  <si>
+    <t>Worked on Philosophy; Curriculum; Rates; Contact Us.  Released v2011.11.04.1</t>
   </si>
 </sst>
 </file>
@@ -399,17 +405,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="110.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -493,18 +499,38 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="4">
-        <f>SUM(B2:B9)</f>
-        <v>570</v>
+      <c r="A8" s="3">
+        <v>40850</v>
+      </c>
+      <c r="B8">
+        <f>3*60</f>
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>40851</v>
+      </c>
+      <c r="B9">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="B11" s="5">
-        <f xml:space="preserve"> (B10/60) * 60</f>
-        <v>570</v>
+      <c r="B11" s="4">
+        <f>SUM(B2:B10)</f>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="5">
+        <f xml:space="preserve"> (B11/60) * 60</f>
+        <v>840</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update images on curriculum and contact us
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Contact Us page got developed and deployed to production</t>
+  </si>
+  <si>
+    <t>Replace images on Curriculum and Contact Us. Released  v.2011.12.05.1</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,16 +539,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="4">
-        <f>SUM(B2:B11)</f>
-        <v>1020</v>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>40882</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="5">
-        <f xml:space="preserve"> (B12/60) * 60</f>
-        <v>1020</v>
+      <c r="B13" s="4">
+        <f>SUM(B2:B12)</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="5">
+        <f xml:space="preserve"> (B13/60) * 60</f>
+        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>